<commit_message>
implémentation déplacement au sein de la grille
</commit_message>
<xml_diff>
--- a/blocs.xlsx
+++ b/blocs.xlsx
@@ -168,7 +168,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -468,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.95" customHeight="1"/>
@@ -2560,7 +2567,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z26">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>